<commit_message>
test and actual excel files are separated
</commit_message>
<xml_diff>
--- a/src/main/resources/biogas-test.xlsx
+++ b/src/main/resources/biogas-test.xlsx
@@ -366,27 +366,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:D11"/>
+  <dimension ref="C4:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6">
         <v>10</v>
       </c>
     </row>
@@ -395,7 +395,7 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <f>D5+D6</f>
+        <f>D4+D5</f>
         <v>20</v>
       </c>
     </row>
@@ -406,6 +406,18 @@
       <c r="D11">
         <f>D10 *5</f>
         <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <f>D74*5</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <f>D4+D5</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>